<commit_message>
Added controller for tables
</commit_message>
<xml_diff>
--- a/RatingUniversity/Files/3_chislennost_pps_vuza.xlsx
+++ b/RatingUniversity/Files/3_chislennost_pps_vuza.xlsx
@@ -1,39 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dilechka\Desktop\last scripts\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
+  <workbookProtection lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
-    <sheet name=" chislennost_pps_vuza" sheetId="1" r:id="rId1"/>
+    <sheet name="chislennost_pps_vuza" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="as_ass">' chislennost_pps_vuza'!$I$9</definedName>
-    <definedName name="as_doz">' chislennost_pps_vuza'!$G$9</definedName>
-    <definedName name="as_fan_doc">' chislennost_pps_vuza'!$E$9</definedName>
-    <definedName name="as_fan_nom">' chislennost_pps_vuza'!$D$9</definedName>
-    <definedName name="as_katta">' chislennost_pps_vuza'!$H$9</definedName>
-    <definedName name="as_prof">' chislennost_pps_vuza'!$F$9</definedName>
-    <definedName name="as_shtat">' chislennost_pps_vuza'!$A$9</definedName>
-    <definedName name="saotbay">' chislennost_pps_vuza'!$C$9</definedName>
-    <definedName name="so_ass">' chislennost_pps_vuza'!$Q$9</definedName>
-    <definedName name="so_doz">' chislennost_pps_vuza'!$O$9</definedName>
-    <definedName name="so_katta">' chislennost_pps_vuza'!$P$9</definedName>
-    <definedName name="so_prof">' chislennost_pps_vuza'!$N$9</definedName>
-    <definedName name="ur_ass">' chislennost_pps_vuza'!$M$9</definedName>
-    <definedName name="ur_doz">' chislennost_pps_vuza'!$K$9</definedName>
-    <definedName name="ur_katta">' chislennost_pps_vuza'!$L$9</definedName>
-    <definedName name="ur_prof">' chislennost_pps_vuza'!$J$9</definedName>
-    <definedName name="urindosh">' chislennost_pps_vuza'!$B$9</definedName>
+    <definedName name="as_ass">chislennost_pps_vuza!$I$9</definedName>
+    <definedName name="as_doz">chislennost_pps_vuza!$G$9</definedName>
+    <definedName name="as_fan_doc">chislennost_pps_vuza!$E$9</definedName>
+    <definedName name="as_fan_nom">chislennost_pps_vuza!$D$9</definedName>
+    <definedName name="as_katta">chislennost_pps_vuza!$H$9</definedName>
+    <definedName name="as_prof">chislennost_pps_vuza!$F$9</definedName>
+    <definedName name="as_shtat">chislennost_pps_vuza!$A$9</definedName>
+    <definedName name="saotbay">chislennost_pps_vuza!$C$9</definedName>
+    <definedName name="so_ass">chislennost_pps_vuza!$Q$9</definedName>
+    <definedName name="so_doz">chislennost_pps_vuza!$O$9</definedName>
+    <definedName name="so_katta">chislennost_pps_vuza!$P$9</definedName>
+    <definedName name="so_prof">chislennost_pps_vuza!$N$9</definedName>
+    <definedName name="ur_ass">chislennost_pps_vuza!$M$9</definedName>
+    <definedName name="ur_doz">chislennost_pps_vuza!$K$9</definedName>
+    <definedName name="ur_katta">chislennost_pps_vuza!$L$9</definedName>
+    <definedName name="ur_prof">chislennost_pps_vuza!$J$9</definedName>
+    <definedName name="urindosh">chislennost_pps_vuza!$B$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Жами</t>
   </si>
@@ -51,9 +47,6 @@
     <t>Профессор-ўқитувчилар сони :</t>
   </si>
   <si>
-    <t>Илмий даражали ва унвонлилар салмоғи, фоизда</t>
-  </si>
-  <si>
     <t>Асосий штатдагилар</t>
   </si>
   <si>
@@ -96,46 +89,20 @@
     <t>доцент</t>
   </si>
   <si>
-    <t>Асосий штатда</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ўриндош </t>
-  </si>
-  <si>
-    <t>Соатбай</t>
-  </si>
-  <si>
-    <t>Жами (биргаликда)</t>
+    <t>ОТМга ажратилган умумий штат сони:</t>
+  </si>
+  <si>
+    <t>* Ташқи ўриндош</t>
+  </si>
+  <si>
+    <t>_____________________________________________</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  да фаолият кўрсатаётган  профессор-ўқитувчилар тўғрисида умумий</t>
   </si>
   <si>
     <r>
-      <t>_____________________________________________</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>да фаолият кўрсатаётган  профессор-ўқитувчилар тўғрисида умумий</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(ОТМ номи)                                                                                           </t>
+      <t xml:space="preserve">                                                 (ОТМ номи)                                                                                           </t>
     </r>
     <r>
       <rPr>
@@ -159,12 +126,6 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
-  </si>
-  <si>
-    <t>ОТМга ажратилган умумий штат сони:</t>
-  </si>
-  <si>
-    <t>* Ташқи ўриндош</t>
   </si>
 </sst>
 </file>
@@ -227,7 +188,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -321,26 +282,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -355,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -377,9 +318,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -401,31 +339,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -443,10 +375,10 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -720,7 +652,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -728,252 +660,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:U13"/>
+  <dimension ref="A2:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="11"/>
-    <col min="4" max="4" width="6.85546875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="11"/>
-    <col min="7" max="7" width="7.5703125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" style="11" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="11" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="11" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="11"/>
-    <col min="13" max="13" width="7" style="11" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="3" width="9.140625" style="10"/>
+    <col min="4" max="4" width="6.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="10"/>
+    <col min="7" max="7" width="7.5703125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="10" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" style="10" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" style="10"/>
+    <col min="13" max="13" width="7" style="10" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
     </row>
-    <row r="3" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
+    <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
     </row>
-    <row r="4" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
+    <row r="4" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
     </row>
-    <row r="5" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="17">
+    <row r="5" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="15">
         <v>0</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
     </row>
-    <row r="6" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+    <row r="6" spans="1:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="22" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="24"/>
+    </row>
+    <row r="8" spans="1:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="23"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="24"/>
     </row>
-    <row r="8" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="25" t="s">
+    <row r="9" spans="1:17" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="24"/>
+      <c r="B9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q9" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="9" spans="1:21" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="N9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="R9" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="S9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="T9" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="U9" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -998,7 +894,7 @@
       <c r="H10" s="1">
         <v>8</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="16">
         <v>9</v>
       </c>
       <c r="J10" s="1">
@@ -1013,7 +909,7 @@
       <c r="M10" s="3">
         <v>13</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="16">
         <v>14</v>
       </c>
       <c r="O10" s="1">
@@ -1022,24 +918,12 @@
       <c r="P10" s="1">
         <v>16</v>
       </c>
-      <c r="Q10" s="18">
+      <c r="Q10" s="16">
         <v>17</v>
       </c>
-      <c r="R10" s="1">
-        <v>18</v>
-      </c>
-      <c r="S10" s="1">
-        <v>19</v>
-      </c>
-      <c r="T10" s="1">
-        <v>20</v>
-      </c>
-      <c r="U10" s="1">
-        <v>21</v>
-      </c>
     </row>
-    <row r="11" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
+    <row r="11" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1047,48 +931,35 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="19"/>
+      <c r="I11" s="17"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="9"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="8"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="4" t="e">
-        <f>$A$11*100/$I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S11" s="4" t="e">
-        <f>$B$11*100/$I$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T11" s="4" t="e">
-        <f>C11*100/I5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U11" s="4" t="e">
-        <f>R11+S11+T11</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="Q11" s="17"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A2:U2"/>
-    <mergeCell ref="A3:U3"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <protectedRanges>
+    <protectedRange sqref="I5" name="Диапазон2"/>
+    <protectedRange sqref="A11:Q11" name="Диапазон1"/>
+  </protectedRanges>
+  <mergeCells count="8">
+    <mergeCell ref="A3:Q3"/>
     <mergeCell ref="D8:I8"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="J8:M8"/>
-    <mergeCell ref="R7:U8"/>
     <mergeCell ref="A7:Q7"/>
     <mergeCell ref="N8:Q8"/>
     <mergeCell ref="A5:H5"/>

</xml_diff>